<commit_message>
RFQ script added in Purchase
</commit_message>
<xml_diff>
--- a/TestDataExcel/ZylerERPPurchase.xlsx
+++ b/TestDataExcel/ZylerERPPurchase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zyler ERP Automation\ZylerERP\TestDataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E0FA27-73B0-4077-AFE4-4F58A0DF43AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6819563-3343-4404-A118-237D064560B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="859" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,9 @@
     <sheet name="InboundTracking" sheetId="8" r:id="rId2"/>
     <sheet name="AccountPayable" sheetId="10" r:id="rId3"/>
     <sheet name="PurchaseOrder" sheetId="6" r:id="rId4"/>
-    <sheet name="Sourcing" sheetId="7" r:id="rId5"/>
-    <sheet name="Customer" sheetId="1" r:id="rId6"/>
+    <sheet name="RFQ" sheetId="14" r:id="rId5"/>
+    <sheet name="Sourcing" sheetId="7" r:id="rId6"/>
+    <sheet name="Customer" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Company</t>
   </si>
@@ -270,6 +271,15 @@
   </si>
   <si>
     <t>Mumbai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fresh Vendor	</t>
+  </si>
+  <si>
+    <t>JO42</t>
+  </si>
+  <si>
+    <t>JO52</t>
   </si>
 </sst>
 </file>
@@ -308,13 +318,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,7 +613,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,7 +837,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,10 +982,83 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBA921D-E84C-4084-94A2-A41433658CDB}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="19.109375" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1500</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03AD2A8F-456B-4983-BD92-08299DCB0EA1}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1164,7 +1250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>

</xml_diff>